<commit_message>
download nuts data to get around the unstable api for the moment
</commit_message>
<xml_diff>
--- a/data/rpdi.xlsx
+++ b/data/rpdi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lancs\homes\06\yusupova\My Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T460p\Documents\R\Housing Observatory\uk-housing-observatory-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6B39C8-6179-488C-AC61-08BBA3A07FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>NT</t>
   </si>
@@ -591,12 +592,15 @@
   </si>
   <si>
     <t>Q3 2018</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -907,16 +911,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O176"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>189</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>0.62990834692897779</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>0.6081474087648514</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1101,7 +1108,7 @@
         <v>0.61974791274913343</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1148,7 +1155,7 @@
         <v>0.60345737186749415</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1195,7 +1202,7 @@
         <v>0.5974760725448296</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>0.58658854881061062</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1289,7 +1296,7 @@
         <v>0.57726203706404144</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1336,7 +1343,7 @@
         <v>0.5541352679473307</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1383,7 +1390,7 @@
         <v>0.53762013995504332</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1430,7 +1437,7 @@
         <v>0.52825407027836568</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1477,7 +1484,7 @@
         <v>0.5330695263696299</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>0.54644089177999733</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>0.55515126791183411</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1618,7 +1625,7 @@
         <v>0.56371815472278641</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1665,7 +1672,7 @@
         <v>0.56512645968838693</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1712,7 +1719,7 @@
         <v>0.56330930135821133</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1759,7 +1766,7 @@
         <v>0.56599626720633656</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1806,7 +1813,7 @@
         <v>0.57196385756290913</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1853,7 +1860,7 @@
         <v>0.5621030202671915</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1900,7 +1907,7 @@
         <v>0.56274072972182732</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1947,7 +1954,7 @@
         <v>0.56186082109189572</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1994,7 +2001,7 @@
         <v>0.56045947617947567</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2041,7 +2048,7 @@
         <v>0.56120820434153784</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2088,7 +2095,7 @@
         <v>0.54718430588488687</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2135,7 +2142,7 @@
         <v>0.5347663880148511</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2182,7 +2189,7 @@
         <v>0.52595664784695928</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2229,7 +2236,7 @@
         <v>0.52554323470098219</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2276,7 +2283,7 @@
         <v>0.51888689628899731</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2323,7 +2330,7 @@
         <v>0.5118560612894173</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>0.51404896580563164</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2417,7 +2424,7 @@
         <v>0.51223709644086202</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2464,7 +2471,7 @@
         <v>0.5072725238338216</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -2511,7 +2518,7 @@
         <v>0.50901707278872443</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -2558,7 +2565,7 @@
         <v>0.5119207749415372</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2605,7 +2612,7 @@
         <v>0.51476067086568611</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2652,7 +2659,7 @@
         <v>0.51740312545152944</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -2699,7 +2706,7 @@
         <v>0.51966256143413159</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -2746,7 +2753,7 @@
         <v>0.52085484823807893</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -2793,7 +2800,7 @@
         <v>0.52560243535043405</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2840,7 +2847,7 @@
         <v>0.53711071933158205</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -2887,7 +2894,7 @@
         <v>0.55303977718592245</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>0.55044396046601962</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -2981,7 +2988,7 @@
         <v>0.55213389183617689</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -3028,7 +3035,7 @@
         <v>0.55952239784523805</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -3075,7 +3082,7 @@
         <v>0.5656436842327307</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -3122,7 +3129,7 @@
         <v>0.57509411136529076</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -3169,7 +3176,7 @@
         <v>0.582853808313755</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -3216,7 +3223,7 @@
         <v>0.5893009069657652</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -3263,7 +3270,7 @@
         <v>0.59124854494404699</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -3310,7 +3317,7 @@
         <v>0.60172080060289379</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -3357,7 +3364,7 @@
         <v>0.61349326137757876</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -3404,7 +3411,7 @@
         <v>0.62500965871082959</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -3451,7 +3458,7 @@
         <v>0.63432023036365548</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -3498,7 +3505,7 @@
         <v>0.64227584685433647</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -3545,7 +3552,7 @@
         <v>0.65652914284323638</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -3592,7 +3599,7 @@
         <v>0.67051731932866387</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -3639,7 +3646,7 @@
         <v>0.67873374024770272</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -3686,7 +3693,7 @@
         <v>0.68672668082669674</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -3733,7 +3740,7 @@
         <v>0.69562972676793933</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3780,7 +3787,7 @@
         <v>0.70694939956166891</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3827,7 +3834,7 @@
         <v>0.72035049859485845</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3874,7 +3881,7 @@
         <v>0.72459120518557629</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -3921,7 +3928,7 @@
         <v>0.72089375713975667</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3968,7 +3975,7 @@
         <v>0.71459127573324854</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -4015,7 +4022,7 @@
         <v>0.71244953606463657</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -4062,7 +4069,7 @@
         <v>0.70411338806119184</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -4109,7 +4116,7 @@
         <v>0.70837403334344873</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -4156,7 +4163,7 @@
         <v>0.7089386615338753</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -4203,7 +4210,7 @@
         <v>0.71015263794034722</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -4250,7 +4257,7 @@
         <v>0.70852904511803994</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -4297,7 +4304,7 @@
         <v>0.70595102557530887</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -4344,7 +4351,7 @@
         <v>0.70362069631432023</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -4391,7 +4398,7 @@
         <v>0.69633143725492752</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -4438,7 +4445,7 @@
         <v>0.70405610783048722</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -4485,7 +4492,7 @@
         <v>0.7089360575748207</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -4532,7 +4539,7 @@
         <v>0.70810783972123814</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -4579,7 +4586,7 @@
         <v>0.712141702374118</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -4626,7 +4633,7 @@
         <v>0.70894690641246205</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -4673,7 +4680,7 @@
         <v>0.71445918643455375</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -4720,7 +4727,7 @@
         <v>0.71484120613414637</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>94</v>
       </c>
@@ -4767,7 +4774,7 @@
         <v>0.71532196008094273</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -4814,7 +4821,7 @@
         <v>0.72160185457142645</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -4861,7 +4868,7 @@
         <v>0.72082390671434626</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>97</v>
       </c>
@@ -4908,7 +4915,7 @@
         <v>0.73257196145221071</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -4955,7 +4962,7 @@
         <v>0.74315457633119986</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -5002,7 +5009,7 @@
         <v>0.7360884365969258</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -5049,7 +5056,7 @@
         <v>0.73579467508344909</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -5096,7 +5103,7 @@
         <v>0.7385031980798118</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -5143,7 +5150,7 @@
         <v>0.74830233111674216</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -5190,7 +5197,7 @@
         <v>0.76480454972229739</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -5237,7 +5244,7 @@
         <v>0.76720622395068605</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>105</v>
       </c>
@@ -5284,7 +5291,7 @@
         <v>0.76261905937528951</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -5331,7 +5338,7 @@
         <v>0.77304864210275515</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>107</v>
       </c>
@@ -5378,7 +5385,7 @@
         <v>0.7916531747364205</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -5425,7 +5432,7 @@
         <v>0.81113334690549022</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -5472,7 +5479,7 @@
         <v>0.81017659242021833</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -5519,7 +5526,7 @@
         <v>0.81016695640675451</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>111</v>
       </c>
@@ -5566,7 +5573,7 @@
         <v>0.83582917090234266</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>112</v>
       </c>
@@ -5613,7 +5620,7 @@
         <v>0.84935975626816695</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>113</v>
       </c>
@@ -5660,7 +5667,7 @@
         <v>0.84850568624249745</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>114</v>
       </c>
@@ -5707,7 +5714,7 @@
         <v>0.84832038390047837</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>115</v>
       </c>
@@ -5754,7 +5761,7 @@
         <v>0.87285719425308483</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>116</v>
       </c>
@@ -5801,7 +5808,7 @@
         <v>0.89709419919227895</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>117</v>
       </c>
@@ -5848,7 +5855,7 @@
         <v>0.908607029987481</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>118</v>
       </c>
@@ -5895,7 +5902,7 @@
         <v>0.92879887906265501</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>119</v>
       </c>
@@ -5942,7 +5949,7 @@
         <v>0.94313655800406959</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>120</v>
       </c>
@@ -5989,7 +5996,7 @@
         <v>0.95030421930182296</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -6036,7 +6043,7 @@
         <v>0.96591433169553587</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>122</v>
       </c>
@@ -6083,7 +6090,7 @@
         <v>0.9648663946506929</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -6130,7 +6137,7 @@
         <v>0.97185509807315762</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>124</v>
       </c>
@@ -6177,7 +6184,7 @@
         <v>0.97118378333003008</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>125</v>
       </c>
@@ -6224,7 +6231,7 @@
         <v>0.96185849486409447</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -6271,7 +6278,7 @@
         <v>0.95860956564546018</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>127</v>
       </c>
@@ -6318,7 +6325,7 @@
         <v>0.98226891404520111</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>128</v>
       </c>
@@ -6365,7 +6372,7 @@
         <v>0.98484912042313877</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>129</v>
       </c>
@@ -6412,7 +6419,7 @@
         <v>0.98490376332660778</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>130</v>
       </c>
@@ -6459,7 +6466,7 @@
         <v>0.99548783036160149</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>131</v>
       </c>
@@ -6506,7 +6513,7 @@
         <v>1.0037450770170295</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>132</v>
       </c>
@@ -6553,7 +6560,7 @@
         <v>1.012991227506951</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>133</v>
       </c>
@@ -6600,7 +6607,7 @@
         <v>1.0090090013162505</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>134</v>
       </c>
@@ -6647,7 +6654,7 @@
         <v>1.0051682397928485</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>135</v>
       </c>
@@ -6694,7 +6701,7 @@
         <v>1.0182770160869914</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>136</v>
       </c>
@@ -6741,7 +6748,7 @@
         <v>1.0255562090817123</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>137</v>
       </c>
@@ -6788,7 +6795,7 @@
         <v>1.0121461650805286</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>138</v>
       </c>
@@ -6835,7 +6842,7 @@
         <v>1.0198831649092968</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>139</v>
       </c>
@@ -6882,7 +6889,7 @@
         <v>1.03495410651318</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>140</v>
       </c>
@@ -6929,7 +6936,7 @@
         <v>1.0364200043642877</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>141</v>
       </c>
@@ -6976,7 +6983,7 @@
         <v>1.038056682456769</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>142</v>
       </c>
@@ -7023,7 +7030,7 @@
         <v>1.0544214786280703</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -7070,7 +7077,7 @@
         <v>1.0534861107563944</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>144</v>
       </c>
@@ -7117,7 +7124,7 @@
         <v>1.0699969347085063</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>145</v>
       </c>
@@ -7164,7 +7171,7 @@
         <v>1.0762036081553705</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>146</v>
       </c>
@@ -7211,7 +7218,7 @@
         <v>1.0835923172646655</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>147</v>
       </c>
@@ -7258,7 +7265,7 @@
         <v>1.0697692928767317</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>148</v>
       </c>
@@ -7305,7 +7312,7 @@
         <v>1.0603754847316105</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -7352,7 +7359,7 @@
         <v>1.0418306419911672</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>150</v>
       </c>
@@ -7399,7 +7406,7 @@
         <v>1.029517493166741</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -7446,7 +7453,7 @@
         <v>1.0542185926350527</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>152</v>
       </c>
@@ -7493,7 +7500,7 @@
         <v>1.053498118054184</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -7540,7 +7547,7 @@
         <v>1.0413951975783338</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>154</v>
       </c>
@@ -7587,7 +7594,7 @@
         <v>1.0213044560579365</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>155</v>
       </c>
@@ -7634,7 +7641,7 @@
         <v>1.0124035462473744</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>156</v>
       </c>
@@ -7681,7 +7688,7 @@
         <v>1.0248498468036578</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>157</v>
       </c>
@@ -7728,7 +7735,7 @@
         <v>1.0043605618159668</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>158</v>
       </c>
@@ -7775,7 +7782,7 @@
         <v>1.0007008045933405</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>159</v>
       </c>
@@ -7822,7 +7829,7 @@
         <v>0.98789701051278533</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>160</v>
       </c>
@@ -7869,7 +7876,7 @@
         <v>0.98351623830363033</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -7916,7 +7923,7 @@
         <v>0.97819886397407707</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>162</v>
       </c>
@@ -7963,7 +7970,7 @@
         <v>0.98141031101429799</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>163</v>
       </c>
@@ -8010,7 +8017,7 @@
         <v>0.99256155725537676</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>164</v>
       </c>
@@ -8057,7 +8064,7 @@
         <v>1.0105758635796749</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>165</v>
       </c>
@@ -8104,7 +8111,7 @@
         <v>1.0016228227286588</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>166</v>
       </c>
@@ -8151,7 +8158,7 @@
         <v>0.98659266800752798</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>167</v>
       </c>
@@ -8198,7 +8205,7 @@
         <v>1.0195295698431497</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>168</v>
       </c>
@@ -8245,7 +8252,7 @@
         <v>1.0268094654987241</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>169</v>
       </c>
@@ -8292,7 +8299,7 @@
         <v>1.0330855489623283</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>170</v>
       </c>
@@ -8339,7 +8346,7 @@
         <v>1.0350573083246266</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>171</v>
       </c>
@@ -8386,7 +8393,7 @@
         <v>1.0355381689475303</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>172</v>
       </c>
@@ -8433,7 +8440,7 @@
         <v>1.0390752835271873</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>173</v>
       </c>
@@ -8480,7 +8487,7 @@
         <v>1.0471540194494737</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>174</v>
       </c>
@@ -8527,7 +8534,7 @@
         <v>1.0525139198451028</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>175</v>
       </c>
@@ -8574,7 +8581,7 @@
         <v>1.0608977030720725</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>176</v>
       </c>
@@ -8621,7 +8628,7 @@
         <v>1.0856325154567754</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>177</v>
       </c>
@@ -8668,7 +8675,7 @@
         <v>1.0750019443447674</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>178</v>
       </c>
@@ -8715,7 +8722,7 @@
         <v>1.0654533758645064</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>179</v>
       </c>
@@ -8762,7 +8769,7 @@
         <v>1.0839244627726863</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>180</v>
       </c>
@@ -8809,7 +8816,7 @@
         <v>1.0956508759541566</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>181</v>
       </c>
@@ -8856,7 +8863,7 @@
         <v>1.0772295704658708</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>182</v>
       </c>
@@ -8903,7 +8910,7 @@
         <v>1.0759965442010981</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>183</v>
       </c>
@@ -8950,7 +8957,7 @@
         <v>1.0868475062354539</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>184</v>
       </c>
@@ -8997,7 +9004,7 @@
         <v>1.0926216423926285</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>185</v>
       </c>
@@ -9044,7 +9051,7 @@
         <v>1.0964917243006285</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>186</v>
       </c>
@@ -9091,7 +9098,7 @@
         <v>1.090471120387182</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>187</v>
       </c>
@@ -9138,7 +9145,7 @@
         <v>1.0914938519101924</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>188</v>
       </c>

</xml_diff>